<commit_message>
Worked on new age excel
Added ages into the new age excel, only 8 ore needed.
</commit_message>
<xml_diff>
--- a/BEAST2/Ptero's/Data/Pterosaur ages_11-23.xlsx
+++ b/BEAST2/Ptero's/Data/Pterosaur ages_11-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revbayes-v1.2.1-win64\revbayes-v1.2.1\Files\PterosaurPhylogeny\BEAST2\Ptero's\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E07A58-31B1-44DE-8847-5E12BEBF11A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F62B7AA-C66D-4986-BCF1-4B29D0CF9C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="138">
   <si>
     <t>Age</t>
   </si>
@@ -363,13 +363,94 @@
     <t>(Martinez et al. 2014)</t>
   </si>
   <si>
-    <t>Caturrita Formation</t>
-  </si>
-  <si>
-    <t>(Bonaparte, Schultz, and Soares 2010)</t>
-  </si>
-  <si>
-    <t>(Zambelli, 1973)</t>
+    <t>Late Carnian</t>
+  </si>
+  <si>
+    <t>Middle Carnian</t>
+  </si>
+  <si>
+    <t>Early Carnian</t>
+  </si>
+  <si>
+    <t>(Langer, Ramezani, and Da Rosa 2018)</t>
+  </si>
+  <si>
+    <t>Linha São Luiz site</t>
+  </si>
+  <si>
+    <t>(Bonaparte, Schultz, and Soares 2010), (Kellner et al. 2022)</t>
+  </si>
+  <si>
+    <t>(Zambelli 1973)</t>
+  </si>
+  <si>
+    <t>(Cabreira et al. 2016)</t>
+  </si>
+  <si>
+    <t>Santa Maria Formation</t>
+  </si>
+  <si>
+    <t>227-230.3</t>
+  </si>
+  <si>
+    <t>230.3-233.6</t>
+  </si>
+  <si>
+    <t>233.6-237</t>
+  </si>
+  <si>
+    <t>(Martínez et al. 2012)</t>
+  </si>
+  <si>
+    <t>(Kammerer et al. 2020)</t>
+  </si>
+  <si>
+    <t>Morondava Basin</t>
+  </si>
+  <si>
+    <t>(Flynn et al. 2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Late Ladinian </t>
+  </si>
+  <si>
+    <t>Late Ladinian</t>
+  </si>
+  <si>
+    <t>Early ladinian</t>
+  </si>
+  <si>
+    <t>Middle Triassic w species</t>
+  </si>
+  <si>
+    <t>237-239.5</t>
+  </si>
+  <si>
+    <t>239.5-242</t>
+  </si>
+  <si>
+    <t>(Marsicano et al. 2016)</t>
+  </si>
+  <si>
+    <t>Chañares Formation</t>
+  </si>
+  <si>
+    <t>(Romer 1971)</t>
+  </si>
+  <si>
+    <t>Ischigualasto Formation</t>
+  </si>
+  <si>
+    <t>Dockum Group &amp; Chinzle Formation</t>
+  </si>
+  <si>
+    <t>(Irmis et al. 2007)</t>
+  </si>
+  <si>
+    <t>(Nesbitt et al. 2009)</t>
+  </si>
+  <si>
+    <t>(Nesbitt et al. 2009)?</t>
   </si>
 </sst>
 </file>
@@ -403,7 +484,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +557,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -504,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -514,7 +607,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -528,6 +621,8 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -811,7 +906,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,7 +982,7 @@
         <v>237</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1109,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C28F51-8982-4167-BE7A-7475AE363CAF}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1121,7 +1216,7 @@
     <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="7" max="7" width="25.77734375" customWidth="1"/>
     <col min="8" max="8" width="37.88671875" customWidth="1"/>
-    <col min="9" max="9" width="28.33203125" customWidth="1"/>
+    <col min="9" max="9" width="31.44140625" customWidth="1"/>
     <col min="10" max="10" width="4.6640625" customWidth="1"/>
     <col min="11" max="11" width="17.88671875" customWidth="1"/>
     <col min="12" max="12" width="21.88671875" customWidth="1"/>
@@ -1419,6 +1514,27 @@
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="13">
+        <v>227</v>
+      </c>
+      <c r="F10" s="15">
+        <v>214.3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" t="s">
+        <v>137</v>
+      </c>
       <c r="K10" t="s">
         <v>72</v>
       </c>
@@ -1433,6 +1549,27 @@
       <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="20">
+        <v>227</v>
+      </c>
+      <c r="F11" s="20">
+        <v>208.5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" t="s">
+        <v>135</v>
+      </c>
+      <c r="I11" t="s">
+        <v>135</v>
+      </c>
       <c r="K11" t="s">
         <v>86</v>
       </c>
@@ -1463,7 +1600,7 @@
         <v>102</v>
       </c>
       <c r="H12" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I12" t="s">
         <v>104</v>
@@ -1476,11 +1613,26 @@
       <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="13">
+        <v>227</v>
+      </c>
+      <c r="F13" s="13">
+        <v>220.8</v>
+      </c>
       <c r="G13" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
+        <v>113</v>
+      </c>
+      <c r="I13" t="s">
+        <v>111</v>
       </c>
       <c r="K13" t="s">
         <v>91</v>
@@ -1496,6 +1648,27 @@
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="15">
+        <v>233.6</v>
+      </c>
+      <c r="F14" s="14">
+        <v>227</v>
+      </c>
+      <c r="G14" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" t="s">
+        <v>120</v>
+      </c>
       <c r="K14" t="s">
         <v>84</v>
       </c>
@@ -1510,6 +1683,27 @@
       <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="C15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="14">
+        <v>239.5</v>
+      </c>
+      <c r="F15" s="13">
+        <v>233.6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>122</v>
+      </c>
+      <c r="H15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I15" t="s">
+        <v>123</v>
+      </c>
       <c r="K15" t="s">
         <v>92</v>
       </c>
@@ -1524,24 +1718,57 @@
       <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="19">
+        <v>236</v>
+      </c>
+      <c r="F16" s="19">
+        <v>234</v>
+      </c>
+      <c r="G16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K17" t="s">
+        <v>108</v>
+      </c>
+      <c r="L17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K18" t="s">
+        <v>109</v>
+      </c>
+      <c r="L18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1566,32 +1793,71 @@
       <c r="I19" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
+        <v>110</v>
+      </c>
+      <c r="L19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="19">
+        <v>231.4</v>
+      </c>
+      <c r="F20" s="14">
+        <v>227</v>
+      </c>
+      <c r="G20" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" t="s">
+        <v>120</v>
+      </c>
+      <c r="I20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K21" t="s">
+        <v>125</v>
+      </c>
+      <c r="L21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K22" t="s">
+        <v>126</v>
+      </c>
+      <c r="L22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>45</v>
       </c>
@@ -1599,7 +1865,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>40</v>
       </c>
@@ -1625,7 +1891,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>100</v>
       </c>
@@ -1633,7 +1899,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Initial run & new xml's
Added the first versions of the new xml's and performed the first run
</commit_message>
<xml_diff>
--- a/BEAST2/Ptero's/Data/Pterosaur ages_11-23.xlsx
+++ b/BEAST2/Ptero's/Data/Pterosaur ages_11-23.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revbayes-v1.2.1-win64\revbayes-v1.2.1\Files\PterosaurPhylogeny\BEAST2\Ptero's\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31285EE9-D13D-44D7-A075-251C41F1670E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53004BED-C3EE-42E3-8A38-587E14173DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defined ages" sheetId="1" r:id="rId1"/>
-    <sheet name="Age bins &amp; Origin age" sheetId="4" r:id="rId2"/>
-    <sheet name="Pterosaurs with ages" sheetId="2" r:id="rId3"/>
-    <sheet name="Median ages &amp; Calibrated ages" sheetId="3" r:id="rId4"/>
+    <sheet name="Pterosaurs with ages" sheetId="2" r:id="rId2"/>
+    <sheet name="Multiple occurences" sheetId="5" r:id="rId3"/>
+    <sheet name="Age bins &amp; Origin age" sheetId="4" r:id="rId4"/>
+    <sheet name="Median ages &amp; Calibrated ages" sheetId="3" r:id="rId5"/>
+    <sheet name="Multiple median" sheetId="7" r:id="rId6"/>
+    <sheet name="Input" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="254">
   <si>
     <t>Age</t>
   </si>
@@ -269,12 +272,6 @@
     <t>Last third of interval</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Layer name</t>
-  </si>
-  <si>
     <t>Seefelder Schichten</t>
   </si>
   <si>
@@ -284,9 +281,6 @@
     <t>(Kellner 2015)</t>
   </si>
   <si>
-    <t>Late Norian?</t>
-  </si>
-  <si>
     <t>(Gasparini, Fernandez, and de la Fuente 2004)</t>
   </si>
   <si>
@@ -311,9 +305,6 @@
     <t>Early Oxfordian</t>
   </si>
   <si>
-    <t>(Wellnhofer 2003)?</t>
-  </si>
-  <si>
     <t>Full interval age:</t>
   </si>
   <si>
@@ -410,18 +401,12 @@
     <t>Ischigualasto Formation</t>
   </si>
   <si>
-    <t>Dockum Group &amp; Chinzle Formation</t>
-  </si>
-  <si>
     <t>(Irmis et al. 2007)</t>
   </si>
   <si>
     <t>(Nesbitt et al. 2009)</t>
   </si>
   <si>
-    <t>(Nesbitt et al. 2009)?</t>
-  </si>
-  <si>
     <t>(Müller et al. 2023)</t>
   </si>
   <si>
@@ -434,9 +419,6 @@
     <t>(Wild 1984)</t>
   </si>
   <si>
-    <t>Zorzino-kalke</t>
-  </si>
-  <si>
     <t>(Stecher 2008)</t>
   </si>
   <si>
@@ -467,18 +449,9 @@
     <t>(Dalla Vecchia 2019)</t>
   </si>
   <si>
-    <t>? (Too many to note one)</t>
-  </si>
-  <si>
     <t>Solnhofen formation</t>
   </si>
   <si>
-    <t>Titonian</t>
-  </si>
-  <si>
-    <t>Blue Lias Formation</t>
-  </si>
-  <si>
     <t>Med Ma</t>
   </si>
   <si>
@@ -536,9 +509,6 @@
     <t>Jurrassic</t>
   </si>
   <si>
-    <t>Early Permian - Ladinian</t>
-  </si>
-  <si>
     <t>Origin time:</t>
   </si>
   <si>
@@ -567,13 +537,280 @@
   </si>
   <si>
     <t>Age seems dodgy</t>
+  </si>
+  <si>
+    <t>accepted_name + number</t>
+  </si>
+  <si>
+    <t>Austriadactylus cristatus - 2</t>
+  </si>
+  <si>
+    <t>Layer/formation name</t>
+  </si>
+  <si>
+    <t>Dromomeron gregorii -2</t>
+  </si>
+  <si>
+    <t>Dromomeron romeri -2</t>
+  </si>
+  <si>
+    <t>Dromomeron romeri -3</t>
+  </si>
+  <si>
+    <t>Austriadactylus cristatus -1</t>
+  </si>
+  <si>
+    <t>Dromomeron gregorii -1</t>
+  </si>
+  <si>
+    <t>Dromomeron romeri -1</t>
+  </si>
+  <si>
+    <t>Dimorphodon macronyx -2</t>
+  </si>
+  <si>
+    <t>Dimorphodon macronyx -1</t>
+  </si>
+  <si>
+    <t>Eudimorphodon ranzii - 1</t>
+  </si>
+  <si>
+    <t>Eudimorphodon ranzii -2</t>
+  </si>
+  <si>
+    <t>Preondactylus buffarinii -1</t>
+  </si>
+  <si>
+    <t>Rhamphorhynchus muensteri - 1</t>
+  </si>
+  <si>
+    <t>Rhamphorhynchus muensteri - 2</t>
+  </si>
+  <si>
+    <t>Zorzino Limestones</t>
+  </si>
+  <si>
+    <t>Zorzino limestones</t>
+  </si>
+  <si>
+    <t>(Wild 1994)</t>
+  </si>
+  <si>
+    <t>(Rigo, TERESA, and Jadoul 2009)</t>
+  </si>
+  <si>
+    <t>(Dalla Vecchia 1995), (Rigo, TERESA, and Jadoul 2009)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Wild 1994), (Rigo, TERESA, and Jadoul 2009) </t>
+  </si>
+  <si>
+    <t>(Vecchia 2019), (Rigo, TERESA, and Jadoul 2009)</t>
+  </si>
+  <si>
+    <t>(Padian 1983)</t>
+  </si>
+  <si>
+    <t>(Cross et al. 2018)</t>
+  </si>
+  <si>
+    <t>Aust Cliff  - Blue lias</t>
+  </si>
+  <si>
+    <t>Questionable source:</t>
+  </si>
+  <si>
+    <t>Unsure of how well the sources fit the formation</t>
+  </si>
+  <si>
+    <t>Unsure formation:</t>
+  </si>
+  <si>
+    <t>Unsure how likely the locality is to be true (Old specimens)</t>
+  </si>
+  <si>
+    <t>(BUCKLAND 1829)</t>
+  </si>
+  <si>
+    <t>(Weedon, Page, and Jenkyns 2019)</t>
+  </si>
+  <si>
+    <t>Early Sinemurian</t>
+  </si>
+  <si>
+    <t>Late Sinemurian</t>
+  </si>
+  <si>
+    <t>199.46-196.18</t>
+  </si>
+  <si>
+    <t>196.18-192.9</t>
+  </si>
+  <si>
+    <t>Lyme Regis - Blue Lias</t>
+  </si>
+  <si>
+    <t>(Schweigert 2000)</t>
+  </si>
+  <si>
+    <t>(Meyer 1839)</t>
+  </si>
+  <si>
+    <t>Early Titonian</t>
+  </si>
+  <si>
+    <t>Sölnhofen formation</t>
+  </si>
+  <si>
+    <t>(Ősi and Prondvai 2009)</t>
+  </si>
+  <si>
+    <t>Late Titonian</t>
+  </si>
+  <si>
+    <t>149.24-146.17</t>
+  </si>
+  <si>
+    <t>146.17-143.1</t>
+  </si>
+  <si>
+    <t>(Schweigert 2007)</t>
+  </si>
+  <si>
+    <t>Dockum Group</t>
+  </si>
+  <si>
+    <t>(Martz and Parker 2017)</t>
+  </si>
+  <si>
+    <t>Chinle Formation</t>
+  </si>
+  <si>
+    <t>(Sarıgül 2016)</t>
+  </si>
+  <si>
+    <t>Dokum Group</t>
+  </si>
+  <si>
+    <t>(Martz and Small 2019)</t>
+  </si>
+  <si>
+    <t>Petrified forest member</t>
+  </si>
+  <si>
+    <t>(Marsh 2018)</t>
+  </si>
+  <si>
+    <t>Rheatian</t>
+  </si>
+  <si>
+    <t>Owl Rock Member</t>
+  </si>
+  <si>
+    <t>Allkaruen_koi</t>
+  </si>
+  <si>
+    <t>Austriadactylus_cristatus</t>
+  </si>
+  <si>
+    <t>Austriadraco_dallavecchiai</t>
+  </si>
+  <si>
+    <t>Cacibupteryx_caribensis</t>
+  </si>
+  <si>
+    <t>Caelestiventus_hanseni</t>
+  </si>
+  <si>
+    <t>Carniadactylus_rosenfeldi</t>
+  </si>
+  <si>
+    <t>Dimorphodon_macronyx</t>
+  </si>
+  <si>
+    <t>Dromomeron_gigas</t>
+  </si>
+  <si>
+    <t>Dromomeron_gregorii</t>
+  </si>
+  <si>
+    <t>Dromomeron_romeri</t>
+  </si>
+  <si>
+    <t>Eudimorphodon_ranzii</t>
+  </si>
+  <si>
+    <t>Faxinalipterus_minimus</t>
+  </si>
+  <si>
+    <t>Ixalerpeton_polesinensis</t>
+  </si>
+  <si>
+    <t>Kongonaphon_kely</t>
+  </si>
+  <si>
+    <t>Lagerpeton_chanarensis</t>
+  </si>
+  <si>
+    <t>Pachagnathus_benitoi</t>
+  </si>
+  <si>
+    <t>Peteinosaurus_zambellii</t>
+  </si>
+  <si>
+    <t>Preondactylus_buffarinii</t>
+  </si>
+  <si>
+    <t>PVSJ_883</t>
+  </si>
+  <si>
+    <t>Raeticodactylus_filisurensis</t>
+  </si>
+  <si>
+    <t>Rhamphorhynchus_muensteri</t>
+  </si>
+  <si>
+    <t>Scleromochlus_taylori_new</t>
+  </si>
+  <si>
+    <t>Seazzadactylus_venieri</t>
+  </si>
+  <si>
+    <t>Venetoraptor_gassenae</t>
+  </si>
+  <si>
+    <t>Yelaphomte_praderioi</t>
+  </si>
+  <si>
+    <t>Austriadactylus_cristatus-2</t>
+  </si>
+  <si>
+    <t>Dromomeron_gregorii-2</t>
+  </si>
+  <si>
+    <t>Dromomeron_romeri-2</t>
+  </si>
+  <si>
+    <t>Dromomeron_romeri-3</t>
+  </si>
+  <si>
+    <t>Dimorphodon_macronyx-2</t>
+  </si>
+  <si>
+    <t>Eudimorphodon_ranzii-2</t>
+  </si>
+  <si>
+    <t>Rhamphorhynchus_muensteri-2</t>
+  </si>
+  <si>
+    <t>Late Permian - Ladinian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +835,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="22">
@@ -693,12 +936,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -724,6 +961,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,7 +998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -784,11 +1027,13 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1074,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1089,10 +1334,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1162,7 +1407,7 @@
         <v>237</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1377,7 +1622,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B22">
         <v>259.55</v>
@@ -1388,113 +1633,145 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
-        <v>158</v>
+      <c r="A25" s="23" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="24" t="s">
+      <c r="A27" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="23" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="24" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>159</v>
-      </c>
-    </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>154</v>
+      <c r="A43" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>153</v>
+      <c r="A44" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -1503,180 +1780,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB01BF7-10C4-4F06-A6FA-A8E8E73C1B53}">
-  <dimension ref="A2:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>259.55</v>
-      </c>
-      <c r="C3">
-        <v>237</v>
-      </c>
-      <c r="D3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E3">
-        <f>B3-143.1</f>
-        <v>116.45000000000002</v>
-      </c>
-      <c r="F3">
-        <f>C3-143.1</f>
-        <v>93.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>237</v>
-      </c>
-      <c r="C4">
-        <v>227.3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E9" si="0">B4-143.1</f>
-        <v>93.9</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F9" si="1">C4-143.1</f>
-        <v>84.200000000000017</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>227.3</v>
-      </c>
-      <c r="C5">
-        <v>209.51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>84.200000000000017</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>66.41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>209.51</v>
-      </c>
-      <c r="C6">
-        <v>201.36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>66.41</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>58.260000000000019</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>201.36</v>
-      </c>
-      <c r="C7">
-        <v>143.1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>58.260000000000019</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B9">
-        <v>259.55</v>
-      </c>
-      <c r="C9">
-        <v>240</v>
-      </c>
-      <c r="D9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>116.45000000000002</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>96.9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C28F51-8982-4167-BE7A-7475AE363CAF}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1690,7 +1798,7 @@
     <col min="9" max="9" width="31.44140625" customWidth="1"/>
     <col min="10" max="10" width="4.6640625" customWidth="1"/>
     <col min="11" max="11" width="17.88671875" customWidth="1"/>
-    <col min="12" max="12" width="21.88671875" customWidth="1"/>
+    <col min="12" max="12" width="49.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -1713,7 +1821,7 @@
         <v>56</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>167</v>
       </c>
       <c r="H1" t="s">
         <v>59</v>
@@ -1745,7 +1853,7 @@
         <v>168.17</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
         <v>62</v>
@@ -1762,7 +1870,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>171</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>28</v>
@@ -1771,22 +1879,22 @@
         <v>72</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E3" s="15">
         <v>217.49</v>
       </c>
-      <c r="F3" s="15">
-        <v>214.03</v>
+      <c r="F3" s="14">
+        <v>209.51</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
         <v>71</v>
       </c>
-      <c r="I3" t="s">
-        <v>76</v>
+      <c r="I3" s="16" t="s">
+        <v>184</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>67</v>
@@ -1803,10 +1911,10 @@
         <v>28</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E4" s="14">
         <v>214.03</v>
@@ -1815,13 +1923,13 @@
         <v>209.51</v>
       </c>
       <c r="G4" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
         <v>78</v>
       </c>
-      <c r="H4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" t="s">
-        <v>90</v>
+      <c r="I4" s="16" t="s">
+        <v>184</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>69</v>
@@ -1838,10 +1946,10 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E5" s="15">
         <v>159.27000000000001</v>
@@ -1850,13 +1958,13 @@
         <v>154.78</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" t="s">
         <v>82</v>
-      </c>
-      <c r="I5" t="s">
-        <v>85</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>68</v>
@@ -1873,7 +1981,7 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -1885,13 +1993,13 @@
         <v>201.36</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>70</v>
@@ -1911,7 +2019,7 @@
         <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E7" s="15">
         <v>217.49</v>
@@ -1920,54 +2028,54 @@
         <v>209.51</v>
       </c>
       <c r="G7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>49</v>
+        <v>175</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>8</v>
+      <c r="D8" s="25" t="s">
+        <v>6</v>
       </c>
       <c r="E8" s="17">
         <v>201.36</v>
       </c>
       <c r="F8" s="17">
-        <v>192.9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>145</v>
+        <v>199.46</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>190</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="I8" t="s">
-        <v>76</v>
-      </c>
-      <c r="K8" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="L8" s="28" t="s">
-        <v>175</v>
+        <v>189</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1978,7 +2086,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1990,51 +2098,60 @@
         <v>201.36</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I9" t="s">
-        <v>101</v>
-      </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
+        <v>97</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>41</v>
+        <v>172</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="13">
+        <v>3</v>
+      </c>
+      <c r="E10" s="20">
+        <f t="shared" ref="E10" si="0">F9</f>
+        <v>201.36</v>
+      </c>
+      <c r="F10" s="20">
         <v>227.3</v>
       </c>
-      <c r="F10" s="15">
-        <v>214.03</v>
-      </c>
       <c r="G10" t="s">
-        <v>123</v>
+        <v>211</v>
       </c>
       <c r="H10" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I10" t="s">
-        <v>126</v>
-      </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
+        <v>212</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="L10" s="29" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>30</v>
@@ -2052,20 +2169,20 @@
         <v>209.51</v>
       </c>
       <c r="G11" t="s">
-        <v>123</v>
+        <v>217</v>
       </c>
       <c r="H11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I11" t="s">
-        <v>124</v>
-      </c>
-      <c r="K11" s="27"/>
-      <c r="L11" s="26"/>
+        <v>119</v>
+      </c>
+      <c r="K11" s="26"/>
+      <c r="L11" s="25"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>38</v>
+        <v>176</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>28</v>
@@ -2074,25 +2191,25 @@
         <v>72</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E12" s="15">
         <v>217.49</v>
       </c>
-      <c r="F12" s="14">
-        <v>209.51</v>
-      </c>
-      <c r="G12" t="s">
-        <v>96</v>
+      <c r="F12" s="15">
+        <v>214.03</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>182</v>
       </c>
       <c r="H12" t="s">
-        <v>107</v>
-      </c>
-      <c r="I12" t="s">
-        <v>98</v>
-      </c>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
+        <v>103</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
@@ -2102,10 +2219,10 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E13" s="12">
         <v>225.42</v>
@@ -2114,16 +2231,16 @@
         <v>217.49</v>
       </c>
       <c r="G13" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I13" t="s">
-        <v>105</v>
-      </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
+        <v>101</v>
+      </c>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
@@ -2132,29 +2249,29 @@
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="E14" s="12">
-        <v>233.2</v>
+      <c r="C14" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="14">
+        <v>233.6</v>
       </c>
       <c r="F14" s="14">
         <v>227.3</v>
       </c>
       <c r="G14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I14" t="s">
-        <v>105</v>
-      </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
+        <v>101</v>
+      </c>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -2164,10 +2281,10 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E15" s="14">
         <v>239.48</v>
@@ -2176,16 +2293,16 @@
         <v>233.6</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I15" t="s">
-        <v>114</v>
-      </c>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
+        <v>110</v>
+      </c>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
@@ -2195,10 +2312,10 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E16" s="19">
         <v>236</v>
@@ -2207,16 +2324,16 @@
         <v>234</v>
       </c>
       <c r="G16" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I16" t="s">
-        <v>119</v>
-      </c>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
+        <v>115</v>
+      </c>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
@@ -2226,7 +2343,7 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -2234,20 +2351,20 @@
       <c r="E17" s="14">
         <v>214.03</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="20">
         <v>201.36</v>
       </c>
       <c r="G17" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I17" t="s">
-        <v>101</v>
-      </c>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
+        <v>97</v>
+      </c>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -2260,7 +2377,7 @@
         <v>72</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E18" s="15">
         <v>217.49</v>
@@ -2269,47 +2386,47 @@
         <v>209.51</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="H18" t="s">
-        <v>130</v>
-      </c>
-      <c r="I18" t="s">
-        <v>76</v>
-      </c>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
+        <v>124</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
+      <c r="A19" s="30" t="s">
+        <v>178</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D19" t="s">
-        <v>87</v>
+      <c r="D19" s="22" t="s">
+        <v>72</v>
       </c>
       <c r="E19" s="15">
         <v>217.49</v>
       </c>
-      <c r="F19" s="14">
-        <v>209.51</v>
-      </c>
-      <c r="G19" t="s">
-        <v>96</v>
+      <c r="F19" s="15">
+        <v>214.03</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="H19" t="s">
-        <v>130</v>
-      </c>
-      <c r="I19" t="s">
-        <v>98</v>
-      </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
+        <v>124</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
@@ -2319,10 +2436,10 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E20" s="19">
         <v>231.4</v>
@@ -2331,16 +2448,16 @@
         <v>227.3</v>
       </c>
       <c r="G20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H20" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I20" t="s">
-        <v>111</v>
-      </c>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
+        <v>107</v>
+      </c>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
@@ -2350,10 +2467,10 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E21" s="14">
         <v>214.03</v>
@@ -2362,47 +2479,48 @@
         <v>205.44</v>
       </c>
       <c r="G21" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="H21" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="I21" t="s">
-        <v>135</v>
-      </c>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
+        <v>128</v>
+      </c>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
     </row>
     <row r="22" spans="1:12" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>52</v>
+        <v>179</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>144</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
-      </c>
-      <c r="E22" s="22">
+        <v>16</v>
+      </c>
+      <c r="E22" s="20">
+        <f>F21</f>
+        <v>205.44</v>
+      </c>
+      <c r="F22" s="20">
         <v>149.24</v>
       </c>
-      <c r="F22" s="22">
-        <v>143.1</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>143</v>
+      <c r="G22" s="28" t="s">
+        <v>135</v>
       </c>
       <c r="H22" t="s">
-        <v>142</v>
+        <v>203</v>
       </c>
       <c r="I22" t="s">
-        <v>76</v>
-      </c>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
+        <v>202</v>
+      </c>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
     </row>
     <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
@@ -2412,10 +2530,10 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E23" s="14">
         <v>233.6</v>
@@ -2424,16 +2542,16 @@
         <v>217.49</v>
       </c>
       <c r="G23" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="H23" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="I23" t="s">
-        <v>138</v>
-      </c>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
+        <v>131</v>
+      </c>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
     </row>
     <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
@@ -2446,7 +2564,7 @@
         <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E24" s="15">
         <v>217.49</v>
@@ -2455,29 +2573,29 @@
         <v>209.51</v>
       </c>
       <c r="G24" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H24" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="I24" t="s">
-        <v>98</v>
-      </c>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
+        <v>94</v>
+      </c>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>102</v>
+      <c r="C25" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>98</v>
       </c>
       <c r="E25" s="14">
         <v>233.6</v>
@@ -2486,16 +2604,16 @@
         <v>227.3</v>
       </c>
       <c r="G25" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H25" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I25" t="s">
-        <v>105</v>
-      </c>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
+        <v>101</v>
+      </c>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
@@ -2505,7 +2623,7 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -2517,24 +2635,24 @@
         <v>201.36</v>
       </c>
       <c r="G26" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H26" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I26" t="s">
-        <v>101</v>
-      </c>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
+        <v>97</v>
+      </c>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F26">
@@ -2544,12 +2662,438 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BF1638-D451-49C3-A187-7D7621821287}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" activeCellId="1" sqref="A2:B8 E2:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
+    <col min="9" max="9" width="36.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="14">
+        <v>214.03</v>
+      </c>
+      <c r="F2" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="20">
+        <v>227.3</v>
+      </c>
+      <c r="F3" s="20">
+        <v>209.51</v>
+      </c>
+      <c r="G3" t="s">
+        <v>215</v>
+      </c>
+      <c r="H3" t="s">
+        <v>214</v>
+      </c>
+      <c r="I3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="15">
+        <v>217.49</v>
+      </c>
+      <c r="F4" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H4" t="s">
+        <v>216</v>
+      </c>
+      <c r="I4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E5" s="20">
+        <f t="shared" ref="E5" si="0">F4</f>
+        <v>209.51</v>
+      </c>
+      <c r="F5" s="20">
+        <v>201.36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>220</v>
+      </c>
+      <c r="H5" t="s">
+        <v>218</v>
+      </c>
+      <c r="I5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" s="17">
+        <v>201.36</v>
+      </c>
+      <c r="F6" s="13">
+        <v>196.18</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="H6" t="s">
+        <v>195</v>
+      </c>
+      <c r="I6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="14">
+        <v>214.03</v>
+      </c>
+      <c r="F7" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>181</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E8" s="13">
+        <v>149.24</v>
+      </c>
+      <c r="F8" s="13">
+        <v>146.16999999999999</v>
+      </c>
+      <c r="G8" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8" t="s">
+        <v>206</v>
+      </c>
+      <c r="I8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB01BF7-10C4-4F06-A6FA-A8E8E73C1B53}">
+  <dimension ref="A2:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>259.55</v>
+      </c>
+      <c r="C3">
+        <v>237</v>
+      </c>
+      <c r="D3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3">
+        <f>B3-143.1</f>
+        <v>116.45000000000002</v>
+      </c>
+      <c r="F3">
+        <f>C3-143.1</f>
+        <v>93.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>237</v>
+      </c>
+      <c r="C4">
+        <v>227.3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E9" si="0">B4-143.1</f>
+        <v>93.9</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F9" si="1">C4-143.1</f>
+        <v>84.200000000000017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>227.3</v>
+      </c>
+      <c r="C5">
+        <v>209.51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>84.200000000000017</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>66.41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>209.51</v>
+      </c>
+      <c r="C6">
+        <v>201.36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>66.41</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>58.260000000000019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>201.36</v>
+      </c>
+      <c r="C7">
+        <v>143.1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>58.260000000000019</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9">
+        <v>259.55</v>
+      </c>
+      <c r="C9">
+        <v>240</v>
+      </c>
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9">
+        <f>B9-146.17</f>
+        <v>113.38000000000002</v>
+      </c>
+      <c r="F9">
+        <f>C9-146.17</f>
+        <v>93.830000000000013</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7518D159-7792-4C0F-A309-DBF9C169F6C8}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2572,16 +3116,16 @@
         <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="H1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2602,16 +3146,16 @@
         <v>172.785</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F21" si="1">E2-143.1</f>
-        <v>29.685000000000002</v>
+        <f>E2-146.17</f>
+        <v>26.615000000000009</v>
       </c>
       <c r="G2">
-        <f>D2-143.1</f>
-        <v>25.069999999999993</v>
+        <f>D2-146.17</f>
+        <v>22</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H21" si="2">C2-143.1</f>
-        <v>34.300000000000011</v>
+        <f>C2-146.17</f>
+        <v>31.230000000000018</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2624,24 +3168,24 @@
       <c r="C3" s="15">
         <v>217.49</v>
       </c>
-      <c r="D3" s="15">
-        <v>214.03</v>
+      <c r="D3" s="14">
+        <v>209.51</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>215.76</v>
+        <v>213.5</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
-        <v>72.66</v>
+        <f t="shared" ref="F3:F26" si="1">E3-146.17</f>
+        <v>67.330000000000013</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G2:G21" si="3">D3-143.1</f>
-        <v>70.930000000000007</v>
+        <f t="shared" ref="G3:G26" si="2">D3-146.17</f>
+        <v>63.34</v>
       </c>
       <c r="H3">
-        <f t="shared" si="2"/>
-        <v>74.390000000000015</v>
+        <f t="shared" ref="H3:H26" si="3">C3-146.17</f>
+        <v>71.320000000000022</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2663,15 +3207,15 @@
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>68.669999999999987</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="G4">
+        <f t="shared" si="2"/>
+        <v>63.34</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="3"/>
-        <v>66.41</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="2"/>
-        <v>70.930000000000007</v>
+        <v>67.860000000000014</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2693,15 +3237,15 @@
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>13.925000000000011</v>
+        <v>10.855000000000018</v>
       </c>
       <c r="G5">
+        <f t="shared" si="2"/>
+        <v>8.6100000000000136</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="3"/>
-        <v>11.680000000000007</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="2"/>
-        <v>16.170000000000016</v>
+        <v>13.100000000000023</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -2723,15 +3267,15 @@
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>64.594999999999999</v>
+        <v>61.525000000000006</v>
       </c>
       <c r="G6">
+        <f t="shared" si="2"/>
+        <v>55.190000000000026</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="3"/>
-        <v>58.260000000000019</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="2"/>
-        <v>70.930000000000007</v>
+        <v>67.860000000000014</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2753,15 +3297,15 @@
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>70.400000000000006</v>
+        <v>67.330000000000013</v>
       </c>
       <c r="G7">
+        <f t="shared" si="2"/>
+        <v>63.34</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="3"/>
-        <v>66.41</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
-        <v>74.390000000000015</v>
+        <v>71.320000000000022</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2775,23 +3319,23 @@
         <v>201.36</v>
       </c>
       <c r="D8" s="17">
-        <v>192.9</v>
+        <v>199.46</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>197.13</v>
+        <v>200.41000000000003</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>54.03</v>
+        <v>54.240000000000038</v>
       </c>
       <c r="G8">
+        <f t="shared" si="2"/>
+        <v>53.29000000000002</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="3"/>
-        <v>49.800000000000011</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
-        <v>58.260000000000019</v>
+        <v>55.190000000000026</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2813,15 +3357,15 @@
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>64.594999999999999</v>
+        <v>61.525000000000006</v>
       </c>
       <c r="G9">
+        <f t="shared" si="2"/>
+        <v>55.190000000000026</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="3"/>
-        <v>58.260000000000019</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>70.930000000000007</v>
+        <v>67.860000000000014</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2831,27 +3375,28 @@
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="20">
+        <f t="shared" ref="C10" si="4">D9</f>
+        <v>201.36</v>
+      </c>
+      <c r="D10" s="20">
         <v>227.3</v>
-      </c>
-      <c r="D10" s="15">
-        <v>214.03</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>220.66500000000002</v>
+        <v>214.33</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>77.565000000000026</v>
+        <v>68.160000000000025</v>
       </c>
       <c r="G10">
+        <f t="shared" si="2"/>
+        <v>81.130000000000024</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="3"/>
-        <v>70.930000000000007</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
-        <v>84.200000000000017</v>
+        <v>55.190000000000026</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2873,15 +3418,15 @@
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>75.305000000000007</v>
+        <v>72.235000000000014</v>
       </c>
       <c r="G11">
+        <f t="shared" si="2"/>
+        <v>63.34</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="3"/>
-        <v>66.41</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
-        <v>84.200000000000017</v>
+        <v>81.130000000000024</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2894,24 +3439,24 @@
       <c r="C12" s="15">
         <v>217.49</v>
       </c>
-      <c r="D12" s="14">
-        <v>209.51</v>
+      <c r="D12" s="15">
+        <v>214.03</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>213.5</v>
+        <v>215.76</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>70.400000000000006</v>
+        <v>69.59</v>
       </c>
       <c r="G12">
+        <f t="shared" si="2"/>
+        <v>67.860000000000014</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="3"/>
-        <v>66.41</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>74.390000000000015</v>
+        <v>71.320000000000022</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2933,15 +3478,15 @@
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>78.35499999999999</v>
+        <v>75.284999999999997</v>
       </c>
       <c r="G13">
+        <f t="shared" si="2"/>
+        <v>71.320000000000022</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="3"/>
-        <v>74.390000000000015</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>82.32</v>
+        <v>79.25</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2951,27 +3496,27 @@
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="12">
-        <v>233.2</v>
+      <c r="C14" s="14">
+        <v>233.6</v>
       </c>
       <c r="D14" s="14">
         <v>227.3</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>230.25</v>
+        <v>230.45</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>87.15</v>
+        <v>84.28</v>
       </c>
       <c r="G14">
+        <f t="shared" si="2"/>
+        <v>81.130000000000024</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="3"/>
-        <v>84.200000000000017</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
-        <v>90.1</v>
+        <v>87.43</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2993,15 +3538,15 @@
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>93.44</v>
+        <v>90.37</v>
       </c>
       <c r="G15">
+        <f t="shared" si="2"/>
+        <v>87.43</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="3"/>
-        <v>90.5</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>96.38</v>
+        <v>93.31</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -3023,15 +3568,15 @@
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>91.9</v>
+        <v>88.830000000000013</v>
       </c>
       <c r="G16">
+        <f t="shared" si="2"/>
+        <v>87.830000000000013</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="3"/>
-        <v>90.9</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="2"/>
-        <v>92.9</v>
+        <v>89.830000000000013</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -3044,7 +3589,7 @@
       <c r="C17" s="14">
         <v>214.03</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="20">
         <v>201.36</v>
       </c>
       <c r="E17">
@@ -3053,15 +3598,15 @@
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>64.594999999999999</v>
+        <v>61.525000000000006</v>
       </c>
       <c r="G17">
+        <f t="shared" si="2"/>
+        <v>55.190000000000026</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="3"/>
-        <v>58.260000000000019</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="2"/>
-        <v>70.930000000000007</v>
+        <v>67.860000000000014</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -3083,15 +3628,15 @@
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>70.400000000000006</v>
+        <v>67.330000000000013</v>
       </c>
       <c r="G18">
+        <f t="shared" si="2"/>
+        <v>63.34</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="3"/>
-        <v>66.41</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="2"/>
-        <v>74.390000000000015</v>
+        <v>71.320000000000022</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -3104,24 +3649,24 @@
       <c r="C19" s="15">
         <v>217.49</v>
       </c>
-      <c r="D19" s="14">
-        <v>209.51</v>
+      <c r="D19" s="15">
+        <v>214.03</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>213.5</v>
+        <v>215.76</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>70.400000000000006</v>
+        <v>69.59</v>
       </c>
       <c r="G19">
+        <f t="shared" si="2"/>
+        <v>67.860000000000014</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="3"/>
-        <v>66.41</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="2"/>
-        <v>74.390000000000015</v>
+        <v>71.320000000000022</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3143,15 +3688,15 @@
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>86.250000000000028</v>
+        <v>83.180000000000035</v>
       </c>
       <c r="G20">
+        <f t="shared" si="2"/>
+        <v>81.130000000000024</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="3"/>
-        <v>84.200000000000017</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="2"/>
-        <v>88.300000000000011</v>
+        <v>85.230000000000018</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3173,15 +3718,15 @@
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>66.635000000000019</v>
+        <v>63.565000000000026</v>
       </c>
       <c r="G21">
+        <f t="shared" si="2"/>
+        <v>59.27000000000001</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="3"/>
-        <v>62.34</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="2"/>
-        <v>70.930000000000007</v>
+        <v>67.860000000000014</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3191,27 +3736,28 @@
       <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="20">
+        <f>D21</f>
+        <v>205.44</v>
+      </c>
+      <c r="D22" s="20">
         <v>149.24</v>
-      </c>
-      <c r="D22" s="22">
-        <v>143.1</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>146.17000000000002</v>
+        <v>177.34</v>
       </c>
       <c r="F22">
-        <f>E22-143.1</f>
+        <f t="shared" si="1"/>
+        <v>31.170000000000016</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
         <v>3.0700000000000216</v>
       </c>
-      <c r="G22">
-        <f>D22-143.1</f>
-        <v>0</v>
-      </c>
       <c r="H22">
-        <f>C22-143.1</f>
-        <v>6.1400000000000148</v>
+        <f t="shared" si="3"/>
+        <v>59.27000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3232,16 +3778,16 @@
         <v>225.54500000000002</v>
       </c>
       <c r="F23">
-        <f t="shared" ref="F23:F26" si="4">E23-143.1</f>
-        <v>82.445000000000022</v>
+        <f t="shared" si="1"/>
+        <v>79.375000000000028</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:G26" si="5">D23-143.1</f>
-        <v>74.390000000000015</v>
+        <f t="shared" si="2"/>
+        <v>71.320000000000022</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:H26" si="6">C23-143.1</f>
-        <v>90.5</v>
+        <f t="shared" si="3"/>
+        <v>87.43</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3262,21 +3808,21 @@
         <v>213.5</v>
       </c>
       <c r="F24">
-        <f t="shared" si="4"/>
-        <v>70.400000000000006</v>
+        <f t="shared" si="1"/>
+        <v>67.330000000000013</v>
       </c>
       <c r="G24">
-        <f t="shared" si="5"/>
-        <v>66.41</v>
+        <f t="shared" si="2"/>
+        <v>63.34</v>
       </c>
       <c r="H24">
-        <f t="shared" si="6"/>
-        <v>74.390000000000015</v>
+        <f t="shared" si="3"/>
+        <v>71.320000000000022</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>30</v>
@@ -3292,16 +3838,16 @@
         <v>230.45</v>
       </c>
       <c r="F25">
-        <f t="shared" si="4"/>
-        <v>87.35</v>
+        <f t="shared" si="1"/>
+        <v>84.28</v>
       </c>
       <c r="G25">
-        <f t="shared" si="5"/>
-        <v>84.200000000000017</v>
+        <f t="shared" si="2"/>
+        <v>81.130000000000024</v>
       </c>
       <c r="H25">
-        <f t="shared" si="6"/>
-        <v>90.5</v>
+        <f t="shared" si="3"/>
+        <v>87.43</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3322,16 +3868,16 @@
         <v>207.69499999999999</v>
       </c>
       <c r="F26">
-        <f t="shared" si="4"/>
-        <v>64.594999999999999</v>
+        <f t="shared" si="1"/>
+        <v>61.525000000000006</v>
       </c>
       <c r="G26">
-        <f t="shared" si="5"/>
-        <v>58.260000000000019</v>
+        <f t="shared" si="2"/>
+        <v>55.190000000000026</v>
       </c>
       <c r="H26">
-        <f t="shared" si="6"/>
-        <v>70.930000000000007</v>
+        <f t="shared" si="3"/>
+        <v>67.860000000000014</v>
       </c>
     </row>
   </sheetData>
@@ -3340,4 +3886,533 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4280E281-9E32-4F6D-A0EF-078B3D4FF18C}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="14">
+        <v>214.03</v>
+      </c>
+      <c r="D2" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2" si="0">(C2+D2)/2</f>
+        <v>211.76999999999998</v>
+      </c>
+      <c r="F2">
+        <f>E2-146.17</f>
+        <v>65.599999999999994</v>
+      </c>
+      <c r="G2">
+        <f>D2-146.17</f>
+        <v>63.34</v>
+      </c>
+      <c r="H2">
+        <f>C2-146.17</f>
+        <v>67.860000000000014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="20">
+        <v>227.3</v>
+      </c>
+      <c r="D3" s="20">
+        <v>209.51</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E8" si="1">(C3+D3)/2</f>
+        <v>218.405</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F8" si="2">E3-146.17</f>
+        <v>72.235000000000014</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G8" si="3">D3-146.17</f>
+        <v>63.34</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H8" si="4">C3-146.17</f>
+        <v>81.130000000000024</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="15">
+        <v>217.49</v>
+      </c>
+      <c r="D4" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>213.5</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>67.330000000000013</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>63.34</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="4"/>
+        <v>71.320000000000022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="20">
+        <v>209.51</v>
+      </c>
+      <c r="D5" s="20">
+        <v>201.36</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>205.435</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>59.265000000000015</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>55.190000000000026</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="4"/>
+        <v>63.34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="17">
+        <v>201.36</v>
+      </c>
+      <c r="D6" s="13">
+        <v>196.18</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>198.77</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>52.600000000000023</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>50.010000000000019</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>55.190000000000026</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="14">
+        <v>214.03</v>
+      </c>
+      <c r="D7" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>211.76999999999998</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>65.599999999999994</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>63.34</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>67.860000000000014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="13">
+        <v>149.24</v>
+      </c>
+      <c r="D8" s="13">
+        <v>146.16999999999999</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>147.70499999999998</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1.5349999999999966</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>3.0700000000000216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F15091-D504-4DDD-8557-0EAD9FA2BD7E}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1">
+        <v>26.615000000000009</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2">
+        <v>67.330000000000013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3">
+        <v>65.599999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4">
+        <v>10.855000000000018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5">
+        <v>61.525000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6">
+        <v>67.330000000000013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7">
+        <v>54.240000000000038</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8">
+        <v>61.525000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9">
+        <v>68.160000000000025</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10">
+        <v>72.235000000000014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11">
+        <v>69.59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12">
+        <v>75.284999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13">
+        <v>84.28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14">
+        <v>90.37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15">
+        <v>88.830000000000013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16">
+        <v>61.525000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17">
+        <v>67.330000000000013</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B18">
+        <v>69.59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B19">
+        <v>83.180000000000035</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20">
+        <v>63.565000000000026</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B21">
+        <v>31.170000000000016</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>242</v>
+      </c>
+      <c r="B22">
+        <v>79.375000000000028</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23">
+        <v>67.330000000000013</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>244</v>
+      </c>
+      <c r="B24">
+        <v>84.28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>245</v>
+      </c>
+      <c r="B25">
+        <v>61.525000000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26">
+        <v>65.599999999999994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B27">
+        <v>72.235000000000014</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B28">
+        <v>67.330000000000013</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B29">
+        <v>59.265000000000015</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B30">
+        <v>52.600000000000023</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B31">
+        <v>65.599999999999994</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated runs with age uncertainty
Added the updated runs with age uncertainty and some of the preliminary runs
</commit_message>
<xml_diff>
--- a/BEAST2/Ptero's/Data/Pterosaur ages_11-23.xlsx
+++ b/BEAST2/Ptero's/Data/Pterosaur ages_11-23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revbayes-v1.2.1-win64\revbayes-v1.2.1\Files\PterosaurPhylogeny\BEAST2\Ptero's\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53004BED-C3EE-42E3-8A38-587E14173DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F620F1E6-BF3B-47E3-A095-01C2CE1BCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defined ages" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Input" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2127,7 +2128,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="20">
-        <f t="shared" ref="E10" si="0">F9</f>
+        <f>F9</f>
         <v>201.36</v>
       </c>
       <c r="F10" s="20">
@@ -2811,7 +2812,7 @@
         <v>219</v>
       </c>
       <c r="E5" s="20">
-        <f t="shared" ref="E5" si="0">F4</f>
+        <f>F4</f>
         <v>209.51</v>
       </c>
       <c r="F5" s="20">
@@ -2923,7 +2924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB01BF7-10C4-4F06-A6FA-A8E8E73C1B53}">
   <dimension ref="A2:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -2965,11 +2966,11 @@
         <v>253</v>
       </c>
       <c r="E3">
-        <f>B3-143.1</f>
+        <f t="shared" ref="E3:F7" si="0">B3-143.1</f>
         <v>116.45000000000002</v>
       </c>
       <c r="F3">
-        <f>C3-143.1</f>
+        <f t="shared" si="0"/>
         <v>93.9</v>
       </c>
     </row>
@@ -2987,11 +2988,11 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E9" si="0">B4-143.1</f>
+        <f t="shared" si="0"/>
         <v>93.9</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F9" si="1">C4-143.1</f>
+        <f t="shared" si="0"/>
         <v>84.200000000000017</v>
       </c>
     </row>
@@ -3013,7 +3014,7 @@
         <v>84.200000000000017</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>66.41</v>
       </c>
     </row>
@@ -3035,7 +3036,7 @@
         <v>66.41</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>58.260000000000019</v>
       </c>
     </row>
@@ -3057,7 +3058,7 @@
         <v>58.260000000000019</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3092,8 +3093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7518D159-7792-4C0F-A309-DBF9C169F6C8}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3376,11 +3377,10 @@
         <v>30</v>
       </c>
       <c r="C10" s="20">
-        <f t="shared" ref="C10" si="4">D9</f>
+        <v>227.3</v>
+      </c>
+      <c r="D10" s="17">
         <v>201.36</v>
-      </c>
-      <c r="D10" s="20">
-        <v>227.3</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
@@ -3392,11 +3392,11 @@
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>81.130000000000024</v>
+        <v>55.190000000000026</v>
       </c>
       <c r="H10">
         <f t="shared" si="3"/>
-        <v>55.190000000000026</v>
+        <v>81.130000000000024</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -3893,7 +3893,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3942,7 +3942,7 @@
         <v>209.51</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2" si="0">(C2+D2)/2</f>
+        <f>(C2+D2)/2</f>
         <v>211.76999999999998</v>
       </c>
       <c r="F2">
@@ -3972,19 +3972,19 @@
         <v>209.51</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E8" si="1">(C3+D3)/2</f>
+        <f t="shared" ref="E3:E8" si="0">(C3+D3)/2</f>
         <v>218.405</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F8" si="2">E3-146.17</f>
+        <f t="shared" ref="F3:F8" si="1">E3-146.17</f>
         <v>72.235000000000014</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G8" si="3">D3-146.17</f>
+        <f t="shared" ref="G3:G8" si="2">D3-146.17</f>
         <v>63.34</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H8" si="4">C3-146.17</f>
+        <f t="shared" ref="H3:H8" si="3">C3-146.17</f>
         <v>81.130000000000024</v>
       </c>
     </row>
@@ -4002,19 +4002,19 @@
         <v>209.51</v>
       </c>
       <c r="E4">
+        <f t="shared" si="0"/>
+        <v>213.5</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="1"/>
-        <v>213.5</v>
-      </c>
-      <c r="F4">
+        <v>67.330000000000013</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="2"/>
-        <v>67.330000000000013</v>
-      </c>
-      <c r="G4">
+        <v>63.34</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="3"/>
-        <v>63.34</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="4"/>
         <v>71.320000000000022</v>
       </c>
     </row>
@@ -4032,19 +4032,19 @@
         <v>201.36</v>
       </c>
       <c r="E5">
+        <f t="shared" si="0"/>
+        <v>205.435</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="1"/>
-        <v>205.435</v>
-      </c>
-      <c r="F5">
+        <v>59.265000000000015</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="2"/>
-        <v>59.265000000000015</v>
-      </c>
-      <c r="G5">
+        <v>55.190000000000026</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="3"/>
-        <v>55.190000000000026</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="4"/>
         <v>63.34</v>
       </c>
     </row>
@@ -4062,19 +4062,19 @@
         <v>196.18</v>
       </c>
       <c r="E6">
+        <f t="shared" si="0"/>
+        <v>198.77</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="1"/>
-        <v>198.77</v>
-      </c>
-      <c r="F6">
+        <v>52.600000000000023</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="2"/>
-        <v>52.600000000000023</v>
-      </c>
-      <c r="G6">
+        <v>50.010000000000019</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="3"/>
-        <v>50.010000000000019</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="4"/>
         <v>55.190000000000026</v>
       </c>
     </row>
@@ -4092,19 +4092,19 @@
         <v>209.51</v>
       </c>
       <c r="E7">
+        <f t="shared" si="0"/>
+        <v>211.76999999999998</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="1"/>
-        <v>211.76999999999998</v>
-      </c>
-      <c r="F7">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="2"/>
-        <v>65.599999999999994</v>
-      </c>
-      <c r="G7">
+        <v>63.34</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="3"/>
-        <v>63.34</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="4"/>
         <v>67.860000000000014</v>
       </c>
     </row>
@@ -4122,19 +4122,19 @@
         <v>146.16999999999999</v>
       </c>
       <c r="E8">
+        <f t="shared" si="0"/>
+        <v>147.70499999999998</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="1"/>
-        <v>147.70499999999998</v>
-      </c>
-      <c r="F8">
+        <v>1.5349999999999966</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="2"/>
-        <v>1.5349999999999966</v>
-      </c>
-      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="4"/>
         <v>3.0700000000000216</v>
       </c>
     </row>
@@ -4147,7 +4147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F15091-D504-4DDD-8557-0EAD9FA2BD7E}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>